<commit_message>
added qol stuff, expanded output & display
</commit_message>
<xml_diff>
--- a/foxholeArtillery/artilleryData.xlsx
+++ b/foxholeArtillery/artilleryData.xlsx
@@ -448,7 +448,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K27"/>
+  <dimension ref="A1:K32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1418,6 +1418,181 @@
         <v>19.93679344171972</v>
       </c>
     </row>
+    <row r="28">
+      <c r="A28" s="2" t="n">
+        <v>26</v>
+      </c>
+      <c r="B28" t="n">
+        <v>254</v>
+      </c>
+      <c r="C28" t="n">
+        <v>2</v>
+      </c>
+      <c r="D28" t="n">
+        <v>173</v>
+      </c>
+      <c r="E28" t="n">
+        <v>4</v>
+      </c>
+      <c r="F28" t="n">
+        <v>124</v>
+      </c>
+      <c r="G28" t="n">
+        <v>4</v>
+      </c>
+      <c r="H28" t="n">
+        <v>324.8198656957328</v>
+      </c>
+      <c r="I28" t="n">
+        <v>4.182947353165744</v>
+      </c>
+      <c r="J28" t="n">
+        <v>409.6172551090812</v>
+      </c>
+      <c r="K28" t="n">
+        <v>502.1897610864444</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="2" t="n">
+        <v>27</v>
+      </c>
+      <c r="B29" t="n">
+        <v>254</v>
+      </c>
+      <c r="C29" t="n">
+        <v>250</v>
+      </c>
+      <c r="D29" t="n">
+        <v>173</v>
+      </c>
+      <c r="E29" t="n">
+        <v>50</v>
+      </c>
+      <c r="F29" t="n">
+        <v>124</v>
+      </c>
+      <c r="G29" t="n">
+        <v>4</v>
+      </c>
+      <c r="H29" t="n">
+        <v>265.5255986927673</v>
+      </c>
+      <c r="I29" t="n">
+        <v>247.1621701919495</v>
+      </c>
+      <c r="J29" t="n">
+        <v>405.4525382353581</v>
+      </c>
+      <c r="K29" t="n">
+        <v>528.89691977809</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="2" t="n">
+        <v>28</v>
+      </c>
+      <c r="B30" t="n">
+        <v>254</v>
+      </c>
+      <c r="C30" t="n">
+        <v>250</v>
+      </c>
+      <c r="D30" t="n">
+        <v>173</v>
+      </c>
+      <c r="E30" t="n">
+        <v>50</v>
+      </c>
+      <c r="F30" t="n">
+        <v>124</v>
+      </c>
+      <c r="G30" t="n">
+        <v>4</v>
+      </c>
+      <c r="H30" t="n">
+        <v>265.5255986927673</v>
+      </c>
+      <c r="I30" t="n">
+        <v>247.1621701919495</v>
+      </c>
+      <c r="J30" t="n">
+        <v>381.5</v>
+      </c>
+      <c r="K30" t="n">
+        <v>87.88171126619655</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="2" t="n">
+        <v>29</v>
+      </c>
+      <c r="B31" t="n">
+        <v>254</v>
+      </c>
+      <c r="C31" t="n">
+        <v>250</v>
+      </c>
+      <c r="D31" t="n">
+        <v>173</v>
+      </c>
+      <c r="E31" t="n">
+        <v>50</v>
+      </c>
+      <c r="F31" t="n">
+        <v>124</v>
+      </c>
+      <c r="G31" t="n">
+        <v>4</v>
+      </c>
+      <c r="H31" t="n">
+        <v>265.5255986927673</v>
+      </c>
+      <c r="I31" t="n">
+        <v>247.1621701919495</v>
+      </c>
+      <c r="J31" t="n">
+        <v>381.5</v>
+      </c>
+      <c r="K31" t="n">
+        <v>87.88171126619655</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="B32" t="n">
+        <v>254</v>
+      </c>
+      <c r="C32" t="n">
+        <v>500</v>
+      </c>
+      <c r="D32" t="n">
+        <v>173</v>
+      </c>
+      <c r="E32" t="n">
+        <v>50</v>
+      </c>
+      <c r="F32" t="n">
+        <v>124</v>
+      </c>
+      <c r="G32" t="n">
+        <v>4</v>
+      </c>
+      <c r="H32" t="n">
+        <v>259.7297935913153</v>
+      </c>
+      <c r="I32" t="n">
+        <v>494.6496505083052</v>
+      </c>
+      <c r="J32" t="n">
+        <v>381.5</v>
+      </c>
+      <c r="K32" t="n">
+        <v>87.88171126619655</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>